<commit_message>
특정 문자 뒤집기 (two pointer algorithm으로 해결)
</commit_message>
<xml_diff>
--- a/src/main/resources/알고리즘 문제 목록.xlsx
+++ b/src/main/resources/알고리즘 문제 목록.xlsx
@@ -5490,7 +5490,29 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>for (String s : sarr) {
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>문자 뒤집을 때도 two pointer algorithm을 사용할 수 있다!!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+for (String s : sarr) {
   char[] carr = s.toCharArray();
   int lt=0, rt=s.length()-1;
   while (lt &lt; rt) {
@@ -5501,6 +5523,7 @@
     rt--;
   }
 }</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -13414,11 +13437,11 @@
         <v>966</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="181.5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" ht="198" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>967</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="13" t="s">
         <v>968</v>
       </c>
     </row>

</xml_diff>

<commit_message>
특정 문자 뒤집기 (Character.isAlphabetic 함수 사용)
</commit_message>
<xml_diff>
--- a/src/main/resources/알고리즘 문제 목록.xlsx
+++ b/src/main/resources/알고리즘 문제 목록.xlsx
@@ -5465,27 +5465,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Character.isLowerCase©
-Character.toUpperCase©
-split("\\s+")
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>sc.next()는 공백이 있을때 끊긴다!!</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>while문을 통한 스트링 반전</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -5523,6 +5502,51 @@
     rt--;
   }
 }</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Character.isLowerCase(c)
+Character.toUpperCase(c)
+Character.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>isAlphabetic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(c)
+split("\\s+")
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sc.next()는 공백이 있을때 끊긴다!!</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -13144,7 +13168,7 @@
   <dimension ref="A3:C57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -13429,20 +13453,20 @@
       </c>
       <c r="B55" s="42"/>
     </row>
-    <row r="56" spans="1:2" ht="66" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>965</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="198" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>966</v>
+      </c>
+      <c r="B57" s="13" t="s">
         <v>967</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>968</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
회문 문자열 (reverse 후 equalIgnoreCase)
</commit_message>
<xml_diff>
--- a/src/main/resources/알고리즘 문제 목록.xlsx
+++ b/src/main/resources/알고리즘 문제 목록.xlsx
@@ -5546,7 +5546,8 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>sc.next()는 공백이 있을때 끊긴다!!</t>
+      <t>sc.next()는 공백이 있을때 끊긴다!!
+s.equalsIgnoreCase()라는 편리한 함수가 있다</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -13168,7 +13169,7 @@
   <dimension ref="A3:C57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -13453,7 +13454,7 @@
       </c>
       <c r="B55" s="42"/>
     </row>
-    <row r="56" spans="1:2" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="99" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>965</v>
       </c>

</xml_diff>

<commit_message>
암호 (Integer.parseInt(num, 2) 를 통한 10진수 변환)
</commit_message>
<xml_diff>
--- a/src/main/resources/알고리즘 문제 목록.xlsx
+++ b/src/main/resources/알고리즘 문제 목록.xlsx
@@ -5534,6 +5534,54 @@
       </rPr>
       <t xml:space="preserve">(c)
 split("\\s+")
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s.replaceAll("[^a-z]", "")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : 부정
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Integer.parseInt(str, 2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : 스트링 2진수를 10진수로 변환해준다!
 </t>
     </r>
     <r>
@@ -13454,7 +13502,7 @@
       </c>
       <c r="B55" s="42"/>
     </row>
-    <row r="56" spans="1:2" ht="99" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="132" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>965</v>
       </c>

</xml_diff>